<commit_message>
add qgis project and update spreadsheet
</commit_message>
<xml_diff>
--- a/data/USAULTIMATECC_FRIDAY.xlsx
+++ b/data/USAULTIMATECC_FRIDAY.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="73">
   <si>
     <t>FIELD</t>
   </si>
@@ -176,6 +176,63 @@
   </si>
   <si>
     <t>CARLETON</t>
+  </si>
+  <si>
+    <t>R1_DIV</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>R2_DIV</t>
+  </si>
+  <si>
+    <t>R3_DIV</t>
+  </si>
+  <si>
+    <t>R4_DIV</t>
+  </si>
+  <si>
+    <t>R5_DIV</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>DARTMOUTH</t>
+  </si>
+  <si>
+    <t>DELAWARE</t>
+  </si>
+  <si>
+    <t>NOTRE DAME</t>
+  </si>
+  <si>
+    <t>FLORIDA</t>
+  </si>
+  <si>
+    <t>CALIFORNIA</t>
+  </si>
+  <si>
+    <t>CAL</t>
+  </si>
+  <si>
+    <t>UCLA</t>
+  </si>
+  <si>
+    <t>TUFTS</t>
+  </si>
+  <si>
+    <t>UCSD</t>
+  </si>
+  <si>
+    <t>TEXAS</t>
+  </si>
+  <si>
+    <t>OHIO STATE</t>
+  </si>
+  <si>
+    <t>VIRGINIA</t>
   </si>
 </sst>
 </file>
@@ -532,107 +589,121 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA14"/>
+  <dimension ref="A1:BF14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B49" sqref="B49"/>
+      <selection pane="topRight" activeCell="X22" sqref="X22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="15.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="15.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="3" customWidth="1"/>
     <col min="8" max="8" width="15.7109375" style="3" customWidth="1"/>
     <col min="9" max="9" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" style="3" customWidth="1"/>
     <col min="11" max="11" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" style="3" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" style="3" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" style="3" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="26.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" style="3" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" style="3" customWidth="1"/>
     <col min="18" max="18" width="15.7109375" style="3" customWidth="1"/>
     <col min="19" max="19" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="15.7109375" style="3" customWidth="1"/>
     <col min="21" max="21" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="3"/>
+    <col min="22" max="22" width="11.5703125" style="3" customWidth="1"/>
+    <col min="23" max="23" width="15.7109375" style="3" customWidth="1"/>
+    <col min="24" max="24" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.7109375" style="3" customWidth="1"/>
+    <col min="26" max="26" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:58" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="V1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
@@ -660,309 +731,674 @@
       <c r="AY1" s="1"/>
       <c r="AZ1" s="1"/>
       <c r="BA1" s="1"/>
+      <c r="BB1" s="1"/>
+      <c r="BC1" s="1"/>
+      <c r="BD1" s="1"/>
+      <c r="BE1" s="1"/>
+      <c r="BF1" s="1"/>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="B2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="3">
+        <v>15</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="3">
+        <v>4</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="3">
-        <v>15</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3">
+        <v>15</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="3">
+      <c r="K2" s="3">
         <v>11</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="L2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="N2" s="3">
+        <v>15</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="P2" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="R2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="O2" s="3">
-        <v>15</v>
-      </c>
-      <c r="P2" s="3" t="s">
+      <c r="S2" s="3">
+        <v>15</v>
+      </c>
+      <c r="T2" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="U2" s="3">
         <v>10</v>
       </c>
+      <c r="V2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="X2" s="3">
+        <v>13</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z2" s="3">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="B3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="3">
+        <v>14</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="3">
+        <v>11</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="3">
+        <v>13</v>
+      </c>
       <c r="J3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="3">
+        <v>11</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="3">
-        <v>15</v>
-      </c>
-      <c r="L3" s="3" t="s">
+      <c r="N3" s="3">
+        <v>15</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="3">
+      <c r="P3" s="3">
         <v>8</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="R3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="3">
-        <v>15</v>
-      </c>
-      <c r="P3" s="3" t="s">
+      <c r="S3" s="3">
+        <v>15</v>
+      </c>
+      <c r="T3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="U3" s="3">
         <v>10</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="V3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="W3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="S3" s="3">
+      <c r="X3" s="3">
         <v>14</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="U3" s="3">
+      <c r="Z3" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="B4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="3">
+        <v>15</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="3">
+        <v>8</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" s="3">
+        <v>15</v>
+      </c>
       <c r="J4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="3">
+        <v>9</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="K4" s="3">
-        <v>15</v>
-      </c>
-      <c r="L4" s="3" t="s">
+      <c r="N4" s="3">
+        <v>15</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M4" s="3">
+      <c r="P4" s="3">
         <v>8</v>
       </c>
+      <c r="Q4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="S4" s="3">
+        <v>10</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="U4" s="3">
+        <v>12</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="X4" s="3">
+        <v>14</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>9</v>
+      </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="B5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="3">
+        <v>15</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="3">
+        <v>3</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="X5" s="3">
+        <v>15</v>
+      </c>
+      <c r="Y5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>13</v>
+      </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="3">
-        <v>15</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="3">
+        <v>15</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="3">
+      <c r="F6" s="3">
         <v>5</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G6" s="3">
+      <c r="I6" s="3">
         <v>14</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="3">
+      <c r="K6" s="3">
         <v>12</v>
       </c>
+      <c r="L6" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="N6" s="3">
+        <v>15</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="P6" s="3">
+        <v>6</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="R6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="S6" s="3">
+        <v>9</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U6" s="3">
+        <v>15</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="W6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="S6" s="3">
-        <v>15</v>
-      </c>
-      <c r="T6" s="3" t="s">
+      <c r="X6" s="3">
+        <v>15</v>
+      </c>
+      <c r="Y6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="U6" s="3">
+      <c r="Z6" s="3">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="3">
-        <v>15</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="3">
+        <v>15</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="3">
+      <c r="F7" s="3">
         <v>7</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G7" s="3">
-        <v>15</v>
-      </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="3">
+        <v>15</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="3">
+      <c r="K7" s="3">
         <v>8</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="L7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="N7" s="3">
+        <v>14</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="P7" s="3">
+        <v>12</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="R7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="3">
+      <c r="S7" s="3">
         <v>12</v>
       </c>
-      <c r="P7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q7" s="3">
+      <c r="T7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="U7" s="3">
         <v>10</v>
       </c>
-      <c r="R7" s="3" t="s">
+      <c r="V7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="W7" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="S7" s="3">
-        <v>15</v>
-      </c>
-      <c r="T7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="U7" s="3">
+      <c r="X7" s="3">
+        <v>15</v>
+      </c>
+      <c r="Y7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z7" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="3">
-        <v>15</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="3">
+        <v>15</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="3">
+      <c r="F8" s="3">
         <v>10</v>
       </c>
+      <c r="G8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="I8" s="3">
+        <v>13</v>
+      </c>
       <c r="J8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="3">
+        <v>11</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="M8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K8" s="3">
-        <v>15</v>
-      </c>
-      <c r="L8" s="3" t="s">
+      <c r="N8" s="3">
+        <v>15</v>
+      </c>
+      <c r="O8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="M8" s="3">
+      <c r="P8" s="3">
         <v>7</v>
       </c>
+      <c r="Q8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="S8" s="3">
+        <v>14</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="U8" s="3">
+        <v>10</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="W8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="X8" s="3">
+        <v>12</v>
+      </c>
+      <c r="Y8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z8" s="3">
+        <v>7</v>
+      </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="3">
-        <v>15</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="3">
+        <v>15</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="3">
+      <c r="F9" s="3">
         <v>10</v>
       </c>
+      <c r="G9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I9" s="3">
+        <v>11</v>
+      </c>
       <c r="J9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="K9" s="3">
+        <v>8</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="M9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K9" s="3">
-        <v>15</v>
-      </c>
-      <c r="L9" s="3" t="s">
+      <c r="N9" s="3">
+        <v>15</v>
+      </c>
+      <c r="O9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="M9" s="3">
+      <c r="P9" s="3">
         <v>8</v>
       </c>
+      <c r="Q9" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="R9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="S9" s="3">
+        <v>15</v>
+      </c>
+      <c r="T9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="U9" s="3">
+        <v>9</v>
+      </c>
+      <c r="V9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="W9" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="S9" s="3">
-        <v>15</v>
-      </c>
-      <c r="T9" s="3" t="s">
+      <c r="X9" s="3">
+        <v>15</v>
+      </c>
+      <c r="Y9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="U9" s="3">
+      <c r="Z9" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="G14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="3">
-        <v>15</v>
-      </c>
-      <c r="H14" s="3" t="s">
+      <c r="I14" s="3">
+        <v>15</v>
+      </c>
+      <c r="J14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I14" s="3">
+      <c r="K14" s="3">
         <v>12</v>
       </c>
-      <c r="N14" s="3" t="s">
+      <c r="L14" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N14" s="3">
+        <v>15</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="P14" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="R14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O14" s="3">
+      <c r="S14" s="3">
         <v>13</v>
       </c>
-      <c r="P14" s="3" t="s">
+      <c r="T14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="Q14" s="3">
+      <c r="U14" s="3">
         <v>14</v>
       </c>
     </row>

</xml_diff>